<commit_message>
The share of categories in expenses and incomes are now visualized.
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politechnikawroclawska-my.sharepoint.com/personal/282223_student_pwr_edu_pl/Documents/Desktop/Programowanie/AllGitHubRepositories/Income and expense analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\OneDrive - Politechnika Wroclawska\Desktop\Programowanie\AllGitHubRepositories\Income and expense analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="657" documentId="8_{98ED9A46-78BA-457A-B64B-06E27D9BD054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6AA4AE9-A375-4276-978B-FF3BB969BA12}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE9C4BE-42E5-462F-8694-877D6F1B4508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DCD49D8-B753-406C-915E-ABC58C62B802}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8337" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8343" uniqueCount="861">
   <si>
     <t>Biedronka</t>
   </si>
@@ -2612,10 +2612,13 @@
     <t>Gift</t>
   </si>
   <si>
-    <t>Math Dep. Govern.</t>
-  </si>
-  <si>
     <t>Electronics</t>
+  </si>
+  <si>
+    <t>Krem do rąk Neutrogena</t>
+  </si>
+  <si>
+    <t>Math.Dep.Govern.</t>
   </si>
 </sst>
 </file>
@@ -2643,7 +2646,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2666,6 +2669,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -2809,7 +2818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2891,31 +2900,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2994,6 +2986,26 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3333,13 +3345,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:I1392" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
-  <autoFilter ref="A1:I1392" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:I1393" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+  <autoFilter ref="A1:I1393" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{90547FFE-E21F-421D-AC45-693600F2C054}" name="Expense date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{1CD334BF-DFC7-48F8-9EBE-DC808B444939}" name="Where bought?" dataDxfId="7"/>
@@ -3347,9 +3355,9 @@
     <tableColumn id="4" xr3:uid="{8178BB77-1C9C-45C0-A7AC-687037F7C3F7}" name="Expense cost" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{FEB7B629-FB8D-4B91-8F6C-AD443A1CC100}" name="Volume unit" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{FBB86F1D-48ED-4CA4-9947-4D7BE2A04671}" name="Volume amount" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{A92DDD11-0D4D-43C3-B239-5115CF39DF23}" name="Expense category" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{D6BC5CBD-767B-4E13-A9D8-7A067188267C}" name="Expense subcategory" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{B32ED791-EE11-4161-88A0-D5AA11B42E62}" name="Payment method" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{A92DDD11-0D4D-43C3-B239-5115CF39DF23}" name="Expense category" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{D6BC5CBD-767B-4E13-A9D8-7A067188267C}" name="Expense subcategory" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{B32ED791-EE11-4161-88A0-D5AA11B42E62}" name="Payment method" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3672,10 +3680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8AB0AA-CBCB-418F-8FB2-09107690DC39}">
-  <dimension ref="A1:I1392"/>
+  <dimension ref="A1:I1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C793" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E843" sqref="E843"/>
+    <sheetView tabSelected="1" topLeftCell="G1126" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L1133" sqref="L1133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4095,9 +4103,9 @@
       <c r="G14" s="24" t="s">
         <v>853</v>
       </c>
-      <c r="H14" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H14" s="8" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Commuting</v>
       </c>
       <c r="I14" s="18" t="s">
         <v>824</v>
@@ -4125,9 +4133,9 @@
       <c r="G15" s="24" t="s">
         <v>852</v>
       </c>
-      <c r="H15" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H15" s="8" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Groceries</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>4</v>
@@ -4155,9 +4163,9 @@
       <c r="G16" s="24" t="s">
         <v>853</v>
       </c>
-      <c r="H16" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H16" s="8" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Commuting</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>824</v>
@@ -4185,9 +4193,9 @@
       <c r="G17" s="24" t="s">
         <v>827</v>
       </c>
-      <c r="H17" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H17" s="8" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Sports</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>824</v>
@@ -4215,9 +4223,9 @@
       <c r="G18" s="24" t="s">
         <v>846</v>
       </c>
-      <c r="H18" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H18" s="8" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Hygiene</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>4</v>
@@ -4245,9 +4253,9 @@
       <c r="G19" s="24" t="s">
         <v>828</v>
       </c>
-      <c r="H19" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H19" s="8" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Housing</v>
       </c>
       <c r="I19" s="18" t="s">
         <v>4</v>
@@ -4304,9 +4312,9 @@
       <c r="G21" s="14" t="s">
         <v>852</v>
       </c>
-      <c r="H21" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H21" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Groceries</v>
       </c>
       <c r="I21" s="18" t="s">
         <v>4</v>
@@ -4334,9 +4342,9 @@
       <c r="G22" s="14" t="s">
         <v>812</v>
       </c>
-      <c r="H22" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H22" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Stationery</v>
       </c>
       <c r="I22" s="18" t="s">
         <v>4</v>
@@ -4364,9 +4372,9 @@
       <c r="G23" s="14" t="s">
         <v>852</v>
       </c>
-      <c r="H23" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H23" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Groceries</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>4</v>
@@ -4394,9 +4402,9 @@
       <c r="G24" s="14" t="s">
         <v>851</v>
       </c>
-      <c r="H24" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H24" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Recreation</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>4</v>
@@ -4424,9 +4432,9 @@
       <c r="G25" s="14" t="s">
         <v>853</v>
       </c>
-      <c r="H25" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H25" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Commuting</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>4</v>
@@ -4483,9 +4491,9 @@
       <c r="G27" s="14" t="s">
         <v>852</v>
       </c>
-      <c r="H27" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H27" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Groceries</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>4</v>
@@ -4513,9 +4521,9 @@
       <c r="G28" s="14" t="s">
         <v>846</v>
       </c>
-      <c r="H28" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H28" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Hygiene</v>
       </c>
       <c r="I28" s="18" t="s">
         <v>4</v>
@@ -4543,9 +4551,9 @@
       <c r="G29" s="14" t="s">
         <v>855</v>
       </c>
-      <c r="H29" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H29" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>DiningOut</v>
       </c>
       <c r="I29" s="18" t="s">
         <v>4</v>
@@ -4573,9 +4581,9 @@
       <c r="G30" s="14" t="s">
         <v>852</v>
       </c>
-      <c r="H30" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H30" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Groceries</v>
       </c>
       <c r="I30" s="18" t="s">
         <v>4</v>
@@ -4603,9 +4611,9 @@
       <c r="G31" s="14" t="s">
         <v>852</v>
       </c>
-      <c r="H31" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H31" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Groceries</v>
       </c>
       <c r="I31" s="18" t="s">
         <v>4</v>
@@ -4633,9 +4641,9 @@
       <c r="G32" s="14" t="s">
         <v>855</v>
       </c>
-      <c r="H32" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H32" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>DiningOut</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>4</v>
@@ -4663,9 +4671,9 @@
       <c r="G33" s="14" t="s">
         <v>853</v>
       </c>
-      <c r="H33" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="H33" s="14" t="str">
+        <f>Expenses[[#This Row],[Expense category]]</f>
+        <v>Commuting</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>4</v>
@@ -6257,7 +6265,7 @@
         <v>1</v>
       </c>
       <c r="G88" s="14" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H88" s="14" t="s">
         <v>93</v>
@@ -6286,7 +6294,7 @@
         <v>1</v>
       </c>
       <c r="G89" s="14" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H89" s="14" t="s">
         <v>95</v>
@@ -29195,7 +29203,7 @@
         <v>1</v>
       </c>
       <c r="G879" s="14" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H879" s="14" t="s">
         <v>533</v>
@@ -34512,8 +34520,8 @@
       <c r="F1062" s="14">
         <v>1</v>
       </c>
-      <c r="G1062" s="14" t="s">
-        <v>858</v>
+      <c r="G1062" s="29" t="s">
+        <v>860</v>
       </c>
       <c r="H1062" s="14" t="s">
         <v>845</v>
@@ -36764,8 +36772,8 @@
       <c r="F1139" s="14">
         <v>1</v>
       </c>
-      <c r="G1139" s="14" t="s">
-        <v>858</v>
+      <c r="G1139" s="29" t="s">
+        <v>860</v>
       </c>
       <c r="H1139" s="14" t="s">
         <v>363</v>
@@ -37579,7 +37587,7 @@
         <v>1</v>
       </c>
       <c r="G1167" s="14" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H1167" s="14" t="s">
         <v>418</v>
@@ -44121,6 +44129,35 @@
         <v>181</v>
       </c>
       <c r="I1392" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1393" s="6">
+        <v>45709</v>
+      </c>
+      <c r="B1393" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1393" s="20" t="s">
+        <v>859</v>
+      </c>
+      <c r="D1393" s="21">
+        <v>-11.99</v>
+      </c>
+      <c r="E1393" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1393" s="20">
+        <v>75</v>
+      </c>
+      <c r="G1393" s="20" t="s">
+        <v>846</v>
+      </c>
+      <c r="H1393" s="20" t="s">
+        <v>611</v>
+      </c>
+      <c r="I1393" s="22" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I've restructured the directory tree. I've created a dataframe which aggregates the average monthly expenses for each category.
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\OneDrive - Politechnika Wroclawska\Desktop\Programowanie\AllGitHubRepositories\Income and expense analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FEA523-BD5C-45D3-AB73-CD6667832B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C31C48-17E9-42CA-A115-7EA0FF176E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DCD49D8-B753-406C-915E-ABC58C62B802}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6961" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6976" uniqueCount="864">
   <si>
     <t>Biedronka</t>
   </si>
@@ -2630,6 +2630,27 @@
   </si>
   <si>
     <t>Product category</t>
+  </si>
+  <si>
+    <t>Książka "Nineteen eighty four"</t>
+  </si>
+  <si>
+    <t>Dostawa przesyłki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dostawa </t>
+  </si>
+  <si>
+    <t>Książka</t>
+  </si>
+  <si>
+    <t>Hubert Górski</t>
+  </si>
+  <si>
+    <t>Gas/benzyna</t>
+  </si>
+  <si>
+    <t>Tankowanie samochodu</t>
   </si>
 </sst>
 </file>
@@ -3246,8 +3267,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:H1395" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A1:H1395" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:H1398" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A1:H1398" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{90547FFE-E21F-421D-AC45-693600F2C054}" name="Expense date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{1CD334BF-DFC7-48F8-9EBE-DC808B444939}" name="Where bought?" dataDxfId="6"/>
@@ -3579,16 +3600,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8AB0AA-CBCB-418F-8FB2-09107690DC39}">
-  <dimension ref="A1:H1395"/>
+  <dimension ref="A1:H1398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1386" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A1396" sqref="A1396:XFD1396"/>
+    <sheetView tabSelected="1" topLeftCell="A309" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C361" sqref="C361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="16.109375" customWidth="1"/>
@@ -34979,7 +35000,7 @@
         <v>1</v>
       </c>
       <c r="G1205" s="12" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="H1205" s="12" t="s">
         <v>652</v>
@@ -39927,6 +39948,84 @@
       </c>
       <c r="H1395" s="17" t="s">
         <v>609</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1396" s="5">
+        <v>45709</v>
+      </c>
+      <c r="B1396" s="16" t="s">
+        <v>861</v>
+      </c>
+      <c r="C1396" s="17" t="s">
+        <v>863</v>
+      </c>
+      <c r="D1396" s="18">
+        <v>26</v>
+      </c>
+      <c r="E1396" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1396" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1396" s="17" t="s">
+        <v>842</v>
+      </c>
+      <c r="H1396" s="17" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1397" s="5">
+        <v>45711</v>
+      </c>
+      <c r="B1397" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1397" s="17" t="s">
+        <v>857</v>
+      </c>
+      <c r="D1397" s="18">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="E1397" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1397" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1397" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1397" s="17" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1398" s="5">
+        <v>45711</v>
+      </c>
+      <c r="B1398" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1398" s="17" t="s">
+        <v>858</v>
+      </c>
+      <c r="D1398" s="18">
+        <v>3.08</v>
+      </c>
+      <c r="E1398" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1398" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1398" s="17" t="s">
+        <v>836</v>
+      </c>
+      <c r="H1398" s="17" t="s">
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -39940,7 +40039,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F4625-7DC1-4913-BB12-ACE71A6709F4}">
-  <dimension ref="A1:A247"/>
+  <dimension ref="A1:A250"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -39951,7 +40050,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A247">_xlfn.UNIQUE(Expenses[Product category])</f>
+        <f t="array" ref="A1:A250">_xlfn.UNIQUE(Expenses[Product category])</f>
         <v>Ser</v>
       </c>
     </row>
@@ -41183,6 +41282,21 @@
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" t="str">
         <v>Rogal</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248" t="str">
+        <v>Gas/benzyna</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249" t="str">
+        <v>Książka</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250" t="str">
+        <v xml:space="preserve">Dostawa </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I've calculated the frequencies of each expense categories for each month and year. I debugged the rounding error.
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\OneDrive - Politechnika Wroclawska\Desktop\Programowanie\AllGitHubRepositories\Income and expense analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C31C48-17E9-42CA-A115-7EA0FF176E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9758DAED-2B33-4BA0-91A8-23D604EF37CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DCD49D8-B753-406C-915E-ABC58C62B802}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3602,8 +3602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8AB0AA-CBCB-418F-8FB2-09107690DC39}">
   <dimension ref="A1:H1398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A309" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C361" sqref="C361"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4287,7 +4287,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
       <c r="D26" s="13">
         <v>9.99</v>

</xml_diff>

<commit_message>
I've plotted the cost distributions
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\OneDrive - Politechnika Wroclawska\Desktop\Programowanie\AllGitHubRepositories\Income and expense analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\OneDrive - Politechnika Wroclawska\Desktop\Programowanie\AllGitHubRepositories\Income-and-expense-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9758DAED-2B33-4BA0-91A8-23D604EF37CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A031A5ED-CDAC-4CA5-A0C1-2EC97C94D0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DCD49D8-B753-406C-915E-ABC58C62B802}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6976" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6991" uniqueCount="866">
   <si>
     <t>Biedronka</t>
   </si>
@@ -2651,6 +2651,12 @@
   </si>
   <si>
     <t>Tankowanie samochodu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PKP </t>
+  </si>
+  <si>
+    <t>Bilet na pociąg Brzeg-Wrocław</t>
   </si>
 </sst>
 </file>
@@ -2791,7 +2797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2861,6 +2867,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3267,8 +3291,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:H1398" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A1:H1398" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:H1401" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A1:H1401" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{90547FFE-E21F-421D-AC45-693600F2C054}" name="Expense date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{1CD334BF-DFC7-48F8-9EBE-DC808B444939}" name="Where bought?" dataDxfId="6"/>
@@ -3600,10 +3624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8AB0AA-CBCB-418F-8FB2-09107690DC39}">
-  <dimension ref="A1:H1398"/>
+  <dimension ref="A1:H1401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="C1395" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H1400" sqref="H1400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40026,6 +40050,85 @@
       </c>
       <c r="H1398" s="17" t="s">
         <v>859</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1399" s="5">
+        <v>45348</v>
+      </c>
+      <c r="B1399" s="16" t="s">
+        <v>864</v>
+      </c>
+      <c r="C1399" s="17" t="s">
+        <v>865</v>
+      </c>
+      <c r="D1399" s="18">
+        <v>-8.33</v>
+      </c>
+      <c r="E1399" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1399" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1399" s="17" t="s">
+        <v>846</v>
+      </c>
+      <c r="H1399" s="17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1400" s="5">
+        <v>45714</v>
+      </c>
+      <c r="B1400" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1400" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1400" s="18">
+        <f>66.99-23-23</f>
+        <v>20.989999999999995</v>
+      </c>
+      <c r="E1400" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1400" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1400" s="17" t="s">
+        <v>823</v>
+      </c>
+      <c r="H1400" s="17" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1401" s="25">
+        <v>45714</v>
+      </c>
+      <c r="B1401" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1401" s="27" t="s">
+        <v>545</v>
+      </c>
+      <c r="D1401" s="28">
+        <v>18</v>
+      </c>
+      <c r="E1401" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1401" s="27">
+        <v>1</v>
+      </c>
+      <c r="G1401" s="29" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1401" s="30" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The saving destination is now typed by user, closed the figures
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\OneDrive - Politechnika Wroclawska\Desktop\Programowanie\AllGitHubRepositories\Income-and-expense-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0A9600-FA26-4DDE-848A-51D80CBAF542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9970616E-ECFF-438C-AE60-2517EA843CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DCD49D8-B753-406C-915E-ABC58C62B802}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6991" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7066" uniqueCount="870">
   <si>
     <t>Biedronka</t>
   </si>
@@ -2657,6 +2657,18 @@
   </si>
   <si>
     <t>Sos sriracha</t>
+  </si>
+  <si>
+    <t>Pierś pieczona</t>
+  </si>
+  <si>
+    <t>Jabłko polskie gala luz</t>
+  </si>
+  <si>
+    <t>Natka</t>
+  </si>
+  <si>
+    <t>Bilet w dwie strony Wrocław-Szklarska poręba</t>
   </si>
 </sst>
 </file>
@@ -2917,6 +2929,47 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -2930,6 +2983,26 @@
           <color auto="1"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2988,11 +3061,10 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3006,84 +3078,9 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+        <bottom style="thin">
           <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3123,146 +3120,6 @@
           <color auto="1"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3327,6 +3184,45 @@
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
       <fill>
         <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
+      <fill>
+        <patternFill patternType="none">
           <fgColor theme="4" tint="0.79998168889431442"/>
           <bgColor auto="1"/>
         </patternFill>
@@ -3345,6 +3241,44 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3408,6 +3342,45 @@
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
           <fgColor theme="4" tint="0.79998168889431442"/>
           <bgColor auto="1"/>
         </patternFill>
@@ -3426,6 +3399,45 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3563,17 +3575,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:H1401" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
-  <autoFilter ref="A1:H1401" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:H1416" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+  <autoFilter ref="A1:H1416" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{90547FFE-E21F-421D-AC45-693600F2C054}" name="Expense date" dataDxfId="15" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{1CD334BF-DFC7-48F8-9EBE-DC808B444939}" name="Where bought?" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{9770A4A3-231B-4D6F-84B9-C11549941152}" name="What bought?" dataDxfId="13" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{8178BB77-1C9C-45C0-A7AC-687037F7C3F7}" name="Expense cost" dataDxfId="12" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{FEB7B629-FB8D-4B91-8F6C-AD443A1CC100}" name="Volume unit" dataDxfId="11" totalsRowDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{FBB86F1D-48ED-4CA4-9947-4D7BE2A04671}" name="Volume amount" dataDxfId="10" totalsRowDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{A92DDD11-0D4D-43C3-B239-5115CF39DF23}" name="Expense category" dataDxfId="9" totalsRowDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{D6BC5CBD-767B-4E13-A9D8-7A067188267C}" name="Product category" dataDxfId="8" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{90547FFE-E21F-421D-AC45-693600F2C054}" name="Expense date" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1CD334BF-DFC7-48F8-9EBE-DC808B444939}" name="Where bought?" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{9770A4A3-231B-4D6F-84B9-C11549941152}" name="What bought?" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{8178BB77-1C9C-45C0-A7AC-687037F7C3F7}" name="Expense cost" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{FEB7B629-FB8D-4B91-8F6C-AD443A1CC100}" name="Volume unit" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{FBB86F1D-48ED-4CA4-9947-4D7BE2A04671}" name="Volume amount" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{A92DDD11-0D4D-43C3-B239-5115CF39DF23}" name="Expense category" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{D6BC5CBD-767B-4E13-A9D8-7A067188267C}" name="Product category" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3896,10 +3908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8AB0AA-CBCB-418F-8FB2-09107690DC39}">
-  <dimension ref="A1:N1401"/>
+  <dimension ref="A1:N1416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A456" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B465" sqref="B465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38760,7 +38772,7 @@
         <v>1</v>
       </c>
       <c r="G1338" s="12" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="H1338" s="12" t="s">
         <v>749</v>
@@ -40333,7 +40345,7 @@
     </row>
     <row r="1399" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1399" s="5">
-        <v>45348</v>
+        <v>45714</v>
       </c>
       <c r="B1399" s="16" t="s">
         <v>863</v>
@@ -40408,6 +40420,396 @@
       </c>
       <c r="H1401" s="17" t="s">
         <v>544</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1402" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1402" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1402" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1402" s="18">
+        <v>4.99</v>
+      </c>
+      <c r="E1402" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1402" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1402" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1402" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1403" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1403" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1403" s="17" t="s">
+        <v>672</v>
+      </c>
+      <c r="D1403" s="18">
+        <v>4.71</v>
+      </c>
+      <c r="E1403" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1403" s="17">
+        <v>450</v>
+      </c>
+      <c r="G1403" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1403" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1404" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1404" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1404" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="D1404" s="18">
+        <v>1.05</v>
+      </c>
+      <c r="E1404" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1404" s="17">
+        <v>100</v>
+      </c>
+      <c r="G1404" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1404" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1405" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1405" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1405" s="17" t="s">
+        <v>734</v>
+      </c>
+      <c r="D1405" s="18">
+        <v>8.99</v>
+      </c>
+      <c r="E1405" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1405" s="17">
+        <v>1000</v>
+      </c>
+      <c r="G1405" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1405" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1406" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1406" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1406" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1406" s="18">
+        <v>14.33</v>
+      </c>
+      <c r="E1406" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1406" s="17">
+        <v>578</v>
+      </c>
+      <c r="G1406" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1406" s="17" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1407" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1407" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1407" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1407" s="18">
+        <v>4.42</v>
+      </c>
+      <c r="E1407" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1407" s="17">
+        <v>340</v>
+      </c>
+      <c r="G1407" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1407" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1408" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1408" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1408" s="17" t="s">
+        <v>866</v>
+      </c>
+      <c r="D1408" s="18">
+        <v>3.49</v>
+      </c>
+      <c r="E1408" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1408" s="17">
+        <v>100</v>
+      </c>
+      <c r="G1408" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1408" s="17" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1409" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1409" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1409" s="17" t="s">
+        <v>865</v>
+      </c>
+      <c r="D1409" s="18">
+        <v>4.49</v>
+      </c>
+      <c r="E1409" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1409" s="17">
+        <v>180</v>
+      </c>
+      <c r="G1409" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1409" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1410" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1410" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1410" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1410" s="18">
+        <v>2.63</v>
+      </c>
+      <c r="E1410" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1410" s="17">
+        <v>755</v>
+      </c>
+      <c r="G1410" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1410" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1411" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1411" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1411" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1411" s="18">
+        <v>1.28</v>
+      </c>
+      <c r="E1411" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1411" s="17">
+        <v>160</v>
+      </c>
+      <c r="G1411" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1411" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1412" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1412" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1412" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1412" s="18">
+        <v>1.99</v>
+      </c>
+      <c r="E1412" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1412" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1412" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1412" s="17" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1413" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1413" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1413" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1413" s="18">
+        <v>2.99</v>
+      </c>
+      <c r="E1413" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1413" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1413" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1413" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1414" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1414" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1414" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1414" s="18">
+        <v>1.98</v>
+      </c>
+      <c r="E1414" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1414" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1414" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1414" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1415" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1415" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1415" s="17" t="s">
+        <v>867</v>
+      </c>
+      <c r="D1415" s="18">
+        <v>3.32</v>
+      </c>
+      <c r="E1415" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1415" s="17">
+        <v>665</v>
+      </c>
+      <c r="G1415" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H1415" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1416" s="5">
+        <v>45716</v>
+      </c>
+      <c r="B1416" s="16" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1416" s="17" t="s">
+        <v>869</v>
+      </c>
+      <c r="D1416" s="18">
+        <v>38</v>
+      </c>
+      <c r="E1416" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1416" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1416" s="17" t="s">
+        <v>841</v>
+      </c>
+      <c r="H1416" s="17" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -40421,7 +40823,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F4625-7DC1-4913-BB12-ACE71A6709F4}">
-  <dimension ref="A1:A250"/>
+  <dimension ref="A1:A251"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -40432,7 +40834,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A250">_xlfn.UNIQUE(Expenses[Product category])</f>
+        <f t="array" ref="A1:A251">_xlfn.UNIQUE(Expenses[Product category])</f>
         <v>Ser</v>
       </c>
     </row>
@@ -41679,6 +42081,11 @@
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" t="str">
         <v xml:space="preserve">Dostawa </v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251" t="str">
+        <v>Natka</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the missing values bug - there can be missing values in both incomes and expenses after we concatenate these dataframes.
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\OneDrive - Politechnika Wroclawska\Desktop\Programowanie\AllGitHubRepositories\Income-and-expense-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9970616E-ECFF-438C-AE60-2517EA843CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F892B96D-A022-41DA-9767-0F16C540DCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DCD49D8-B753-406C-915E-ABC58C62B802}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7066" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7071" uniqueCount="872">
   <si>
     <t>Biedronka</t>
   </si>
@@ -2669,6 +2669,12 @@
   </si>
   <si>
     <t>Bilet w dwie strony Wrocław-Szklarska poręba</t>
+  </si>
+  <si>
+    <t>Bilet na warsztaty</t>
+  </si>
+  <si>
+    <t>Bilet na warsztaty integracyjne</t>
   </si>
 </sst>
 </file>
@@ -3575,8 +3581,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:H1416" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
-  <autoFilter ref="A1:H1416" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}" name="Expenses" displayName="Expenses" ref="A1:H1417" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+  <autoFilter ref="A1:H1417" xr:uid="{27298FF8-4A57-420C-B73C-701132E4C37B}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{90547FFE-E21F-421D-AC45-693600F2C054}" name="Expense date" dataDxfId="15" totalsRowDxfId="14"/>
     <tableColumn id="2" xr3:uid="{1CD334BF-DFC7-48F8-9EBE-DC808B444939}" name="Where bought?" dataDxfId="13" totalsRowDxfId="12"/>
@@ -3908,25 +3914,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8AB0AA-CBCB-418F-8FB2-09107690DC39}">
-  <dimension ref="A1:N1416"/>
+  <dimension ref="A1:N1417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B465" sqref="B465"/>
+    <sheetView tabSelected="1" topLeftCell="A1407" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1417" sqref="A1417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="1" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" customWidth="1"/>
+    <col min="8" max="8" width="27.88671875" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -40810,6 +40816,32 @@
       </c>
       <c r="H1416" s="17" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1417" s="5">
+        <v>45717</v>
+      </c>
+      <c r="B1417" s="16" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1417" s="17" t="s">
+        <v>871</v>
+      </c>
+      <c r="D1417" s="18">
+        <v>25</v>
+      </c>
+      <c r="E1417" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1417" s="17">
+        <v>1</v>
+      </c>
+      <c r="G1417" s="17" t="s">
+        <v>843</v>
+      </c>
+      <c r="H1417" s="17" t="s">
+        <v>870</v>
       </c>
     </row>
   </sheetData>
@@ -40823,7 +40855,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F4625-7DC1-4913-BB12-ACE71A6709F4}">
-  <dimension ref="A1:A251"/>
+  <dimension ref="A1:A252"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -40834,7 +40866,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A251">_xlfn.UNIQUE(Expenses[Product category])</f>
+        <f t="array" ref="A1:A252">_xlfn.UNIQUE(Expenses[Product category])</f>
         <v>Ser</v>
       </c>
     </row>
@@ -42086,6 +42118,11 @@
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" t="str">
         <v>Natka</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252" t="str">
+        <v>Bilet na warsztaty</v>
       </c>
     </row>
   </sheetData>

</xml_diff>